<commit_message>
add new data to statistic
</commit_message>
<xml_diff>
--- a/history/общий 25.03_тиньков.xlsx
+++ b/history/общий 25.03_тиньков.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavel.rostov\PycharmProjects\scrapyBotTrade\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavel.rostov\PycharmProjects\scrapyBotTrade\history\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F3F93C-E3B2-4682-8F89-9C0812CF2EB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4E59B6-EA11-4115-8F85-27592602EF9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1786,7 +1786,7 @@
   <dimension ref="A1:CR431"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="CR62" sqref="CR62"/>
+      <selection activeCell="CU91" sqref="CU91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -1814,9 +1814,8 @@
     <col min="72" max="76" width="0" hidden="1" customWidth="1" outlineLevel="2"/>
     <col min="77" max="77" width="9.140625" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="78" max="80" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="81" max="85" width="0" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="86" max="86" width="9.140625" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="87" max="89" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="81" max="85" width="9.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="86" max="89" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="90" max="90" width="9.140625" collapsed="1"/>
   </cols>
   <sheetData>

</xml_diff>